<commit_message>
Frontend: update pages and API for PBL6
</commit_message>
<xml_diff>
--- a/frontend/KTPM_PHU/DataTest/Login.xlsx
+++ b/frontend/KTPM_PHU/DataTest/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\Medical-Store-frontend\Medical-Store-frontend\frontend\KTPM_PHU\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A134E34-22F7-4F1F-BD24-C519422FBB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30973557-F374-4F02-AB21-307BA9848624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4668" yWindow="2904" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Data" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>